<commit_message>
Atualizando o backlog de requisitos
</commit_message>
<xml_diff>
--- a/Site/Documentação/Documentação ALL/6tracker - BacklogRequisitos.xlsx
+++ b/Site/Documentação/Documentação ALL/6tracker - BacklogRequisitos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="142">
   <si>
     <t>Requisitos 6Tracker</t>
   </si>
@@ -383,14 +383,140 @@
     <t xml:space="preserve">Relatório e Análises </t>
   </si>
   <si>
-    <t>Inserção de dados no banco</t>
+    <t>Tratamento de dados</t>
+  </si>
+  <si>
+    <t>O tratamento será feito e no MySQL</t>
+  </si>
+  <si>
+    <t>Não funcional</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Importa o CSV da tabela "RAW" do MySQL, excluindo valores nulos, tranformando bytes em Mega e/ou Giga, realizando um cruzamento de informações e gerar um gráfico baseado nisso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruzamento de informações </t>
+  </si>
+  <si>
+    <t>Restrições e acessos</t>
+  </si>
+  <si>
+    <t>Processador e REDE - visualizar como o ato tráfego na REDE afeta no desempenho da CPU.</t>
+  </si>
+  <si>
+    <t>Hierarquia de cadastros realizada no banco MySQL onde os funcionários tem acesso de visualização e os usuários administradores em acesso de visualização e gerenciamento no cadastro dos funcionários.</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t>Requisição de dados no banco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site programado </t>
+  </si>
+  <si>
+    <t>Aplicação de Monitoramento</t>
+  </si>
+  <si>
+    <t>Aplicação de Kotlin</t>
+  </si>
+  <si>
+    <t>Aplicação em Python</t>
+  </si>
+  <si>
+    <t>O banco de dados será feito no MysSQL.</t>
+  </si>
+  <si>
+    <t>O banco armazena as informações da empresa, funcionários e servidores rastredos (através do NodeJs).</t>
+  </si>
+  <si>
+    <t>O banco fornece os dados de hardware para serem enviados para a dashboard (através do NodeJs).</t>
+  </si>
+  <si>
+    <t>O Site será feito em HTML com modulações visuais feitas em CSS e funcionalidades executadas com JavaScript e NodeJs (detalhadamente acima).</t>
+  </si>
+  <si>
+    <t>A aplicação, será feita em Kotlin, Python e Java de forma aa ser um executável.</t>
+  </si>
+  <si>
+    <t>Captura os dados de IP (pra confirmação), rede (download e upload) em Mb com data e hora, e insere no banco de dados na tabela "Dados capturados".</t>
+  </si>
+  <si>
+    <t>Captura os dados de IP  (para inserção na tabela "Servidor"), Disco em Gigabytes, Processador em porcentagem e memória RAM em Megabytes inserindo no banco de dados na tabela "Dados capturados"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela com Painel de Gráficos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plotação de gráficos </t>
+  </si>
+  <si>
+    <t>Exportação dos dados pro gráfico</t>
+  </si>
+  <si>
+    <t>Tela de ADM</t>
+  </si>
+  <si>
+    <t>Logoff</t>
+  </si>
+  <si>
+    <t>Página onde poderá ser visto, em gráficos, a utilização dos componentes de hardware e software, assim fazendo o acompanhamento do monitoramento (Dashboard).</t>
+  </si>
+  <si>
+    <t>Gráficos exibidos na dashboard em porcentagem de uso da CPU, uso de memória RAM em Gb, uso de Rede em Mb e uso de disco em Gb.</t>
+  </si>
+  <si>
+    <t>Os dados são transportados do banco MySQL para os gráficos da dashboard através do NodeJS.</t>
+  </si>
+  <si>
+    <t>Nesta tela, o usuário administrador (hierarquia alta) poderá ter acesso as informações cadastradas de cada funcionário, além de poder visualizar, cadastrar, editar e excluir se necessário.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botão para o usuário se deslogar e sair da parte de gerenciamento, voltando para a parte institucional do site. </t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Tamanho (número)</t>
+  </si>
+  <si>
+    <t>Grande</t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grande </t>
+  </si>
+  <si>
+    <t>médio</t>
+  </si>
+  <si>
+    <t>Pequeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserção de dados no banco </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +527,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -495,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -509,6 +643,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,13 +661,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -813,10 +956,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="G2:L46"/>
+  <dimension ref="G2:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,19 +970,26 @@
     <col min="10" max="10" width="26.140625" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="14" width="11.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G2" s="5" t="s">
+    <row r="2" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
@@ -858,8 +1008,15 @@
       <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="7:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="O3" s="11"/>
+    </row>
+    <row r="4" spans="7:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="2">
         <v>1</v>
       </c>
@@ -878,8 +1035,14 @@
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="7:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="M4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="7:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G5" s="2">
         <v>2</v>
       </c>
@@ -898,8 +1061,14 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="7:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="M5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="7:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G6" s="2">
         <v>3</v>
       </c>
@@ -918,8 +1087,14 @@
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="M6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N6" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G7" s="2">
         <v>4</v>
       </c>
@@ -938,8 +1113,14 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="M7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G8" s="2">
         <v>5</v>
       </c>
@@ -958,8 +1139,14 @@
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="7:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="M8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N8" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="7:18" ht="60" x14ac:dyDescent="0.25">
       <c r="G9" s="2">
         <v>6</v>
       </c>
@@ -978,8 +1165,14 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="7:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="M9" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="7:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G10" s="2">
         <v>7</v>
       </c>
@@ -998,8 +1191,14 @@
       <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="M10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N10" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G11" s="2">
         <v>8</v>
       </c>
@@ -1018,8 +1217,14 @@
       <c r="L11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="7:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="M11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N11" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="7:18" ht="60" x14ac:dyDescent="0.25">
       <c r="G12" s="2">
         <v>9</v>
       </c>
@@ -1038,8 +1243,14 @@
       <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="7:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="M12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N12" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G13" s="2">
         <v>10</v>
       </c>
@@ -1058,8 +1269,14 @@
       <c r="L13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="7:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="M13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N13" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="7:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G14" s="2">
         <v>11</v>
       </c>
@@ -1078,8 +1295,14 @@
       <c r="L14" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="7:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N14" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="7:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="G15" s="2">
         <v>12</v>
       </c>
@@ -1098,8 +1321,10 @@
       <c r="L15" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="7:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="7:18" ht="75" x14ac:dyDescent="0.25">
       <c r="G16" s="2">
         <v>13</v>
       </c>
@@ -1118,8 +1343,14 @@
       <c r="L16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="7:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="M16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" ht="60" x14ac:dyDescent="0.25">
       <c r="G17" s="2">
         <v>14</v>
       </c>
@@ -1138,8 +1369,14 @@
       <c r="L17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="7:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="M17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" ht="75" x14ac:dyDescent="0.25">
       <c r="G18" s="2">
         <v>15</v>
       </c>
@@ -1158,8 +1395,14 @@
       <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N18" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="7:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="G19" s="2">
         <v>16</v>
       </c>
@@ -1178,8 +1421,10 @@
       <c r="L19" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="7:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M19"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="7:14" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="G20" s="2">
         <v>17</v>
       </c>
@@ -1198,8 +1443,10 @@
       <c r="L20" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="7:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="M20"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="7:14" ht="135" x14ac:dyDescent="0.25">
       <c r="G21" s="1">
         <v>18</v>
       </c>
@@ -1218,8 +1465,14 @@
       <c r="L21" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="7:12" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N21" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="G22" s="1">
         <v>19</v>
       </c>
@@ -1238,8 +1491,10 @@
       <c r="L22" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="7:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M22"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="7:14" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="G23" s="1">
         <v>20</v>
       </c>
@@ -1258,8 +1513,10 @@
       <c r="L23" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M23"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="7:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="G24" s="1">
         <v>21</v>
       </c>
@@ -1278,8 +1535,10 @@
       <c r="L24" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="7:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="M24"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="7:14" ht="105" x14ac:dyDescent="0.25">
       <c r="G25" s="1">
         <v>22</v>
       </c>
@@ -1298,8 +1557,14 @@
       <c r="L25" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="7:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="M25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N25" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="7:14" ht="75" x14ac:dyDescent="0.25">
       <c r="G26" s="1">
         <v>23</v>
       </c>
@@ -1318,8 +1583,14 @@
       <c r="L26" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="7:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="M26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N26" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="7:14" ht="120" x14ac:dyDescent="0.25">
       <c r="G27" s="1">
         <v>24</v>
       </c>
@@ -1338,8 +1609,14 @@
       <c r="L27" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="7:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="M27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N27" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="7:14" ht="105" x14ac:dyDescent="0.25">
       <c r="G28" s="1">
         <v>25</v>
       </c>
@@ -1358,8 +1635,14 @@
       <c r="L28" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="7:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="M28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N28" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="7:14" ht="105" x14ac:dyDescent="0.25">
       <c r="G29" s="1">
         <v>26</v>
       </c>
@@ -1378,8 +1661,14 @@
       <c r="L29" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="7:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="M29" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N29" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="7:14" ht="75" x14ac:dyDescent="0.25">
       <c r="G30" s="1">
         <v>27</v>
       </c>
@@ -1396,10 +1685,16 @@
         <v>9</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="7:12" ht="90" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N30" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="7:14" ht="90" x14ac:dyDescent="0.25">
       <c r="G31" s="1">
         <v>28</v>
       </c>
@@ -1418,8 +1713,14 @@
       <c r="L31" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="7:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="M31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N31" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="7:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="1">
         <v>29</v>
       </c>
@@ -1438,8 +1739,14 @@
       <c r="L32" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="7:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M32" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N32" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="2">
         <v>30</v>
       </c>
@@ -1458,8 +1765,14 @@
       <c r="L33" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M33" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N33" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G34" s="2">
         <v>31</v>
       </c>
@@ -1478,8 +1791,14 @@
       <c r="L34" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N34" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G35" s="2">
         <v>32</v>
       </c>
@@ -1498,8 +1817,14 @@
       <c r="L35" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M35" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N35" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G36" s="2">
         <v>33</v>
       </c>
@@ -1518,8 +1843,14 @@
       <c r="L36" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M36" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N36" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G37" s="2">
         <v>34</v>
       </c>
@@ -1538,8 +1869,14 @@
       <c r="L37" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M37" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N37" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G38" s="2">
         <v>35</v>
       </c>
@@ -1558,8 +1895,14 @@
       <c r="L38" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N38" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="7:14" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G39" s="2">
         <v>36</v>
       </c>
@@ -1578,8 +1921,14 @@
       <c r="L39" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M39" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N39" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G40" s="2">
         <v>37</v>
       </c>
@@ -1598,8 +1947,14 @@
       <c r="L40" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="7:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M40" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N40" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G41" s="2">
         <v>39</v>
       </c>
@@ -1618,8 +1973,14 @@
       <c r="L41" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M41" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N41" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="7:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G42" s="2">
         <v>40</v>
       </c>
@@ -1638,8 +1999,14 @@
       <c r="L42" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N42" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="7:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G43" s="2">
         <v>41</v>
       </c>
@@ -1658,8 +2025,14 @@
       <c r="L43" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="7:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M43" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N43" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="7:14" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G44" s="2">
         <v>42</v>
       </c>
@@ -1678,8 +2051,14 @@
       <c r="L44" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="7:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M44" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N44" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="7:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G45" s="2">
         <v>43</v>
       </c>
@@ -1698,17 +2077,431 @@
       <c r="L45" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="7:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="G46" s="8">
+      <c r="M45" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N45" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G46" s="5">
         <v>30</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="H46" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="I46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N46" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="7:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="G47" s="6">
+        <v>70</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N47" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="7:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G48" s="6">
+        <v>89</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N48" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="7:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="G49" s="6">
+        <v>76</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N49" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G50" s="6">
+        <v>73</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N50" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="7:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="G51" s="6">
+        <v>79</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N51" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="7:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G52" s="6">
+        <v>65</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N52" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="7:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="G53" s="6">
+        <v>63</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N53" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="7:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G54" s="6">
+        <v>99</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N54" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="7:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="G55" s="6">
+        <v>96</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N55" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="7:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="G56" s="6">
+        <v>69</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N56" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="7:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="G57" s="6">
+        <v>76</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N57" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="7:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="G58" s="6">
+        <v>81</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N58" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="7:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G59" s="6">
+        <v>92</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N59" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="7:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="G60" s="6">
+        <v>64</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N60" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="G61" s="6">
+        <v>59</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N61" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N62" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="G3:L45">
@@ -1719,7 +2512,7 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="G2:R2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>